<commit_message>
Minor changes due to unsaved tests
</commit_message>
<xml_diff>
--- a/1Homework/DataBase/users.xlsx
+++ b/1Homework/DataBase/users.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaip\Desktop\EXCEL DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Desarrollo Web Duodécimo\Programación para web\PRIMER SEMESTRE\1 TAREA\1Homework\1Homework\DataBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12F3455-C251-456A-9BEC-5B68C173459A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CD5D36-96AD-4EA4-8E8E-FD37FC17C9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -363,13 +363,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>